<commit_message>
Task 03 Api val ent rep
Api automation task 03 until reporting
Validations
Entity
Reporting
</commit_message>
<xml_diff>
--- a/reports/excel/my_xlsx_report.xlsx
+++ b/reports/excel/my_xlsx_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,17 +483,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test_get_all_users</t>
+          <t>test_get_all_posts</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Test get all user from GET endpoint</t>
+          <t>Test get all posts from GET endpoint</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,17 +502,17 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.4855373000027612</v>
+        <v>43.73259660002077</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-04-11T10:26:45</t>
+          <t>2024-04-11T17:52:58</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>test_get_user</t>
+          <t>test_get_post</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Test get a specific user from GET endpoint</t>
+          <t>Test get a specific post from GET endpoint</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -543,39 +543,39 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.4904726999811828</v>
+        <v>0.4714413000037894</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-04-11T10:26:46</t>
+          <t>2024-04-11T17:52:58</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>sanity</t>
+          <t>acceptance</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>test_create_user</t>
+          <t>test_create_post</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Test create a new user (post method)</t>
+          <t>Test create a new post (posts method)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -584,17 +584,17 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>43.09059419995174</v>
+        <v>44.12231100001372</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-04-11T10:27:29</t>
+          <t>2024-04-11T17:53:42</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -606,17 +606,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>test_update_user</t>
+          <t>test_update_post</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Test update user (the last created)</t>
+          <t>Test update post (the last created)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -625,17 +625,17 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.9344848000328057</v>
+        <v>1.392656399984844</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-04-11T10:27:30</t>
+          <t>2024-04-11T17:53:44</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -647,17 +647,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>test_delete_user</t>
+          <t>test_delete_post</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Test delete a user</t>
+          <t>Test delete a post</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -666,20 +666,225 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.070477599976584</v>
+        <v>1.414252799993847</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-04-11T10:27:31</t>
+          <t>2024-04-11T17:53:45</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
+          <t>gorest_api\posts\test_posts.py</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>test_get_all_users</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Test get all user from GET endpoint</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>43.03381850000005</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-04-11T17:55:12</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>gorest_api\users\test_users.py</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>test_get_user</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Test get a specific user from GET endpoint</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4369194000028074</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-04-11T17:55:13</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>sanity</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>test_create_user</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Test create a new user (posts method)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6174863000051118</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-04-11T17:55:13</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>test_update_user</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Test update user (the last created)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1.045363800018094</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-04-11T17:55:14</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>test_delete_user</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Test delete a user</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1.008605799986981</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024-04-11T17:55:15</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>acceptance</t>
         </is>

</xml_diff>

<commit_message>
Task 03 running other reports
Updating missing last report files.
reason:
PyCharm issue: slow performace machine
</commit_message>
<xml_diff>
--- a/reports/excel/my_xlsx_report.xlsx
+++ b/reports/excel/my_xlsx_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,11 +502,11 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>43.73259660002077</v>
+        <v>43.60830139997415</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-04-11T17:52:58</t>
+          <t>2024-04-14T00:12:38</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -543,11 +543,11 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.4714413000037894</v>
+        <v>0.4832969999988563</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-04-11T17:52:58</t>
+          <t>2024-04-14T00:12:38</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -584,11 +584,11 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>44.12231100001372</v>
+        <v>43.53136759999325</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-04-11T17:53:42</t>
+          <t>2024-04-14T00:13:22</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -625,11 +625,11 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.392656399984844</v>
+        <v>1.498724299977766</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-04-11T17:53:44</t>
+          <t>2024-04-14T00:13:23</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -666,11 +666,11 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.414252799993847</v>
+        <v>1.463173900003312</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-04-11T17:53:45</t>
+          <t>2024-04-14T00:13:25</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -707,11 +707,11 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>43.03381850000005</v>
+        <v>42.97459470000467</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-04-11T17:55:12</t>
+          <t>2024-04-14T00:14:52</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -748,11 +748,11 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.4369194000028074</v>
+        <v>0.4309544999850914</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-04-11T17:55:13</t>
+          <t>2024-04-14T00:14:52</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -789,11 +789,11 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.6174863000051118</v>
+        <v>0.4897482999949716</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-04-11T17:55:13</t>
+          <t>2024-04-14T00:14:53</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -830,11 +830,11 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1.045363800018094</v>
+        <v>0.9210826000198722</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-04-11T17:55:14</t>
+          <t>2024-04-14T00:14:54</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -871,11 +871,11 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.008605799986981</v>
+        <v>1.028996900015045</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-04-11T17:55:15</t>
+          <t>2024-04-14T00:14:55</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -887,6 +887,129 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>test_required_field_name</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Test required field is not sent in request body (name)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0.4375171000137925</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2024-04-14T00:14:55</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>test_email_already_taken</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Test email address is already taken</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9908925000054296</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024-04-14T00:14:56</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>test_nonexistent_user</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Test trying to retrieve a user that does not exist</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0.435685900010867</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2024-04-14T00:14:56</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>negative</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates on feature files
Feature files updates
</commit_message>
<xml_diff>
--- a/reports/excel/my_xlsx_report.xlsx
+++ b/reports/excel/my_xlsx_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,11 +502,11 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1.015777099999923</v>
+        <v>1.190232500011916</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:05</t>
+          <t>2024-05-07T13:26:54</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -534,7 +534,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Test get a specific post from GET endpoint</t>
+          <t>Test get a specific post object from GET endpoint</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -543,11 +543,11 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.4245240999998714</v>
+        <v>0.540167900006054</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:05</t>
+          <t>2024-05-07T13:26:55</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -575,7 +575,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Test create a new post (posts method)</t>
+          <t>Test create a new post object (posts method)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -584,11 +584,11 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1.551110599999902</v>
+        <v>1.937018500000704</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:07</t>
+          <t>2024-05-07T13:26:57</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -616,7 +616,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Test update post (the last created)</t>
+          <t>Test update post object (the last created)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -625,11 +625,11 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.404759000000013</v>
+        <v>1.737903000001097</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:08</t>
+          <t>2024-05-07T13:26:58</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -666,11 +666,11 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.418933500000094</v>
+        <v>1.653955000001588</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:10</t>
+          <t>2024-05-07T13:27:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -688,17 +688,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>test_get_all_users</t>
+          <t>test_required_title</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Test get all user from GET endpoint</t>
+          <t>Test title required field is not sent in request body</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -707,39 +707,39 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1.046083100000033</v>
+        <v>0.5037437000137288</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:13</t>
+          <t>2024-05-07T13:27:01</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>acceptance</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>test_get_user</t>
+          <t>test_required_body</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Test get a specific user from GET endpoint</t>
+          <t>Test body required field is not sent in request body</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -748,39 +748,39 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.4709462999999232</v>
+        <v>0.5080416999990121</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:14</t>
+          <t>2024-05-07T13:27:01</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>sanity</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestPosts</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>test_create_user</t>
+          <t>test_nonexistent_post</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Test create a new user (posts method)</t>
+          <t>Test trying to retrieve a post object that does not exist</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -789,39 +789,39 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.5407816000001731</v>
+        <v>0.5132924999925308</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:14</t>
+          <t>2024-05-07T13:27:02</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\posts\test_posts.py</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>acceptance</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestTodos</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>test_update_user</t>
+          <t>test_get_all_todos</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Test update user (the last created)</t>
+          <t>Test get all todos from GET endpoint</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -830,17 +830,17 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1.0036384</v>
+        <v>1.336760799997137</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:15</t>
+          <t>2024-05-07T13:27:05</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\todos\test_todos.py</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -852,17 +852,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestTodos</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>test_delete_user</t>
+          <t>test_get_todo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Test delete a user</t>
+          <t>Test get a specific todos object from GET endpoint</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -871,17 +871,17 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.9941186999999445</v>
+        <v>0.600476499996148</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:16</t>
+          <t>2024-05-07T13:27:06</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\todos\test_todos.py</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -893,17 +893,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestTodos</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>test_required_field_name</t>
+          <t>test_create_todo</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Test required field is not sent in request body (name)</t>
+          <t>Test create a new todo_object (posts method)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -912,39 +912,39 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.4375958999999057</v>
+        <v>1.858424400008516</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:17</t>
+          <t>2024-05-07T13:27:08</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\todos\test_todos.py</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>acceptance</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestTodos</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>test_email_already_taken</t>
+          <t>test_update_todo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Test email address is already taken</t>
+          <t>Test update todo_object (the last created)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -953,39 +953,39 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.9910890999999538</v>
+        <v>1.790401999998721</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:18</t>
+          <t>2024-05-07T13:27:10</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>gorest_api\users\test_users.py</t>
+          <t>gorest_api\todos\test_todos.py</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>acceptance</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TestUsers</t>
+          <t>TestTodos</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>test_nonexistent_user</t>
+          <t>test_delete_todo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Test trying to retrieve a user that does not exist</t>
+          <t>Test delete a todo_object</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -994,20 +994,348 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.4332086999997955</v>
+        <v>1.737185999998474</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2024-04-19T14:06:18</t>
+          <t>2024-05-07T13:27:11</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
+          <t>gorest_api\todos\test_todos.py</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>test_get_all_users</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Test get all user from GET endpoint</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1.26391720000538</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:16</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>gorest_api\users\test_users.py</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>test_get_user</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Test get a specific user from GET endpoint</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0.5325499000027776</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:16</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>sanity</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>test_create_user</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Test create a new user (posts method)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0.643302099997527</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:17</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>test_update_user</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Test update user (the last created)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1.218064999993658</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:18</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>test_delete_user</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Test delete a user</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>1.453652500000317</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:20</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>acceptance</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>test_required_field_name</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Test required field is not sent in request body (name)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0.5441369000036502</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:20</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>test_email_already_taken</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Test email address is already taken</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>1.17042070000025</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:21</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>TestUsers</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>test_nonexistent_user</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Test trying to retrieve a user that does not exist</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0.529216400012956</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2024-05-07T13:27:22</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>gorest_api\users\test_users.py</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>negative</t>
         </is>

</xml_diff>